<commit_message>
Change expand por tag
</commit_message>
<xml_diff>
--- a/Definicion Lenguaje/Definicion-Lenguaje.xlsx
+++ b/Definicion Lenguaje/Definicion-Lenguaje.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://estudianteccr-my.sharepoint.com/personal/stsandoval_estudiantec_cr/Documents/Semestre V/Compiladores e Intérpretes/Proyecto/Notch Engine/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Desktop\Ing. Computacion\1 - Semestres\2025 - 1 semestre\Compiladores\Proyecto\Compiladores\Definicion Lenguaje\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="723" documentId="8_{0E548644-266F-4A7E-B59C-5679FFF401CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AEC37B20-C849-41B1-B597-7DA0ACA04600}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5685DC5-E2D2-417C-9BD1-846166EC4249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" xr2:uid="{01E84666-E791-4DD0-9963-66505EB533A8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{01E84666-E791-4DD0-9963-66505EB533A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Definición del Lenguaje" sheetId="2" r:id="rId1"/>
@@ -566,9 +566,6 @@
   </si>
   <si>
     <t>Tipo de dato número flotante</t>
-  </si>
-  <si>
-    <t>unlock, lock, make, gather, forge, expand</t>
   </si>
   <si>
     <t>spawner &lt;instrucciones&gt; exhausted &lt;cond&gt; ;</t>
@@ -588,6 +585,9 @@
       </rPr>
       <t>.ne</t>
     </r>
+  </si>
+  <si>
+    <t>unlock, lock, make, gather, forge, tag</t>
   </si>
 </sst>
 </file>
@@ -906,18 +906,18 @@
     <cellStyle name="Accent 1" xfId="2" xr:uid="{7A2D3686-E81D-407C-8105-9BB2A515DCA5}"/>
     <cellStyle name="Accent 2" xfId="3" xr:uid="{CD87B413-D703-40A8-B508-348BE407238C}"/>
     <cellStyle name="Accent 3" xfId="4" xr:uid="{A1878133-184C-44BC-B09C-AD6729A1A59F}"/>
-    <cellStyle name="Bad" xfId="5" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Bueno" xfId="8" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Encabezado 1" xfId="10" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Error" xfId="6" xr:uid="{E5C43F8E-7E65-4939-A41A-35BAB2CB0882}"/>
     <cellStyle name="Footnote" xfId="7" xr:uid="{36CB60FB-D47C-4374-B381-AACBA002D798}"/>
-    <cellStyle name="Good" xfId="8" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading" xfId="9" xr:uid="{B1CF2686-0075-42AE-8DC5-574179E89825}"/>
-    <cellStyle name="Heading 1" xfId="10" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Incorrecto" xfId="5" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="12" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="13" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Notas" xfId="13" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Status" xfId="14" xr:uid="{115248D7-D654-4027-BFAB-5ACD55499DC3}"/>
     <cellStyle name="Text" xfId="15" xr:uid="{99B0EB63-7DBB-4B3E-8810-FB7FF6301FC3}"/>
+    <cellStyle name="Título 2" xfId="11" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Warning" xfId="16" xr:uid="{18A2E88A-72BB-4B08-B7AF-E9607373CDF5}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1068,7 +1068,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1386,29 +1386,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46E6B535-EEEA-48F6-947D-F56200620491}">
   <dimension ref="B3:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20" defaultRowHeight="24.9" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="1"/>
-    <col min="2" max="2" width="5.28515625" style="17" customWidth="1"/>
-    <col min="3" max="3" width="50.140625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="61.5703125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="69.7109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" style="17" customWidth="1"/>
+    <col min="3" max="3" width="50.109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="61.5546875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="69.6640625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" s="2" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:5" s="2" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="17"/>
       <c r="C3" s="3"/>
       <c r="D3" s="8"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="2:5" ht="111.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:5" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="4"/>
     </row>
-    <row r="6" spans="2:5" s="1" customFormat="1" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" s="1" customFormat="1" ht="36.6" x14ac:dyDescent="0.3">
       <c r="B6" s="17">
         <v>1</v>
       </c>
@@ -1419,16 +1419,16 @@
         <v>94</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="B7" s="17"/>
       <c r="C7" s="11"/>
       <c r="D7" s="12"/>
       <c r="E7" s="10"/>
     </row>
-    <row r="8" spans="2:5" s="13" customFormat="1" ht="22.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:5" s="13" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="B8" s="17"/>
       <c r="C8" s="7" t="s">
         <v>0</v>
@@ -1436,7 +1436,7 @@
       <c r="D8" s="12"/>
       <c r="E8" s="9"/>
     </row>
-    <row r="9" spans="2:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B9" s="17">
         <v>2</v>
       </c>
@@ -1450,7 +1450,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="2:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B10" s="17">
         <v>3</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="11" spans="2:5" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" s="1" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="B11" s="17">
         <v>4</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="12" spans="2:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B12" s="17">
         <v>5</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="13" spans="2:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B13" s="17">
         <v>6</v>
       </c>
@@ -1506,7 +1506,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="14" spans="2:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B14" s="17">
         <v>7</v>
       </c>
@@ -1520,7 +1520,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="15" spans="2:5" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5" s="1" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="B15" s="17">
         <v>8</v>
       </c>
@@ -1534,7 +1534,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="16" spans="2:5" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B16" s="17">
         <v>9</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="17" spans="2:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B17" s="17">
         <v>10</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="2:5" s="1" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" s="1" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="B18" s="17">
         <v>11</v>
       </c>
@@ -1576,7 +1576,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="2:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B19" s="17">
         <v>12</v>
       </c>
@@ -1590,7 +1590,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="20" spans="2:5" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" s="1" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="B20" s="17">
         <v>13</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="21" spans="2:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B21" s="17">
         <v>14</v>
       </c>
@@ -1618,7 +1618,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="22" spans="2:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B22" s="17">
         <v>15</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="23" spans="2:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B23" s="17">
         <v>16</v>
       </c>
@@ -1646,7 +1646,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="24" spans="2:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B24" s="17">
         <v>17</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="25" spans="2:5" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B25" s="17">
         <v>18</v>
       </c>
@@ -1674,7 +1674,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="26" spans="2:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B26" s="17">
         <v>19</v>
       </c>
@@ -1688,7 +1688,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="27" spans="2:5" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" s="1" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="B27" s="17">
         <v>20</v>
       </c>
@@ -1702,7 +1702,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="28" spans="2:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B28" s="17">
         <v>21</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="2:5" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" s="1" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="B29" s="17">
         <v>22</v>
       </c>
@@ -1730,7 +1730,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="2:5" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" s="1" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="B30" s="17">
         <v>23</v>
       </c>
@@ -1744,7 +1744,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="31" spans="2:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B31" s="17">
         <v>24</v>
       </c>
@@ -1758,7 +1758,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="32" spans="2:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B32" s="17">
         <v>25</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="33" spans="2:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B33" s="17">
         <v>26</v>
       </c>
@@ -1786,7 +1786,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="34" spans="2:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B34" s="17">
         <v>27</v>
       </c>
@@ -1800,7 +1800,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="35" spans="2:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B35" s="17">
         <v>28</v>
       </c>
@@ -1814,7 +1814,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="36" spans="2:5" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B36" s="17">
         <v>29</v>
       </c>
@@ -1828,7 +1828,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="37" spans="2:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B37" s="17">
         <v>30</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="38" spans="2:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B38" s="17">
         <v>31</v>
       </c>
@@ -1856,7 +1856,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="39" spans="2:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B39" s="17">
         <v>32</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="40" spans="2:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B40" s="17">
         <v>33</v>
       </c>
@@ -1884,7 +1884,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="41" spans="2:5" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:5" s="1" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="B41" s="17">
         <v>34</v>
       </c>
@@ -1898,7 +1898,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="42" spans="2:5" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:5" s="1" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="B42" s="17">
         <v>35</v>
       </c>
@@ -1912,7 +1912,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="43" spans="2:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B43" s="17">
         <v>36</v>
       </c>
@@ -1926,7 +1926,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="44" spans="2:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B44" s="17">
         <v>37</v>
       </c>
@@ -1940,7 +1940,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="45" spans="2:5" s="1" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:5" s="1" customFormat="1" ht="52.2" x14ac:dyDescent="0.3">
       <c r="B45" s="17">
         <v>38</v>
       </c>
@@ -1954,7 +1954,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="46" spans="2:5" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B46" s="17">
         <v>39</v>
       </c>
@@ -1968,7 +1968,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="47" spans="2:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B47" s="17">
         <v>40</v>
       </c>
@@ -1976,13 +1976,13 @@
         <v>18</v>
       </c>
       <c r="D47" s="10" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="E47" s="10" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="48" spans="2:5" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B48" s="17">
         <v>41</v>
       </c>
@@ -1996,7 +1996,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="49" spans="2:5" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B49" s="17">
         <v>42</v>
       </c>
@@ -2010,7 +2010,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="50" spans="2:5" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:5" s="1" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="B50" s="17">
         <v>43</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="51" spans="2:5" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B51" s="17">
         <v>44</v>
       </c>
@@ -2038,7 +2038,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="52" spans="2:5" s="1" customFormat="1" ht="72" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:5" s="1" customFormat="1" ht="52.2" x14ac:dyDescent="0.3">
       <c r="B52" s="17">
         <v>45</v>
       </c>
@@ -2052,7 +2052,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="53" spans="2:5" s="1" customFormat="1" ht="72" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:5" s="1" customFormat="1" ht="52.2" x14ac:dyDescent="0.3">
       <c r="B53" s="17">
         <v>46</v>
       </c>
@@ -2066,7 +2066,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="54" spans="2:5" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:5" s="1" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="B54" s="17">
         <v>47</v>
       </c>
@@ -2074,13 +2074,13 @@
         <v>24</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E54" s="10" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="55" spans="2:5" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:5" s="1" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="B55" s="17">
         <v>48</v>
       </c>
@@ -2094,7 +2094,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="56" spans="2:5" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B56" s="17">
         <v>49</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="57" spans="2:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B57" s="17">
         <v>50</v>
       </c>
@@ -2120,7 +2120,7 @@
       </c>
       <c r="E57" s="10"/>
     </row>
-    <row r="58" spans="2:5" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:5" s="1" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="B58" s="17">
         <v>51</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="59" spans="2:5" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:5" s="1" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="B59" s="17">
         <v>52</v>
       </c>
@@ -2148,7 +2148,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="60" spans="2:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B60" s="17">
         <v>53</v>
       </c>
@@ -2160,7 +2160,7 @@
       </c>
       <c r="E60" s="10"/>
     </row>
-    <row r="61" spans="2:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B61" s="17">
         <v>54</v>
       </c>
@@ -2172,7 +2172,7 @@
       </c>
       <c r="E61" s="10"/>
     </row>
-    <row r="62" spans="2:5" s="1" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:5" s="1" customFormat="1" ht="52.2" x14ac:dyDescent="0.3">
       <c r="B62" s="17">
         <v>55</v>
       </c>
@@ -2186,7 +2186,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="63" spans="2:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B63" s="17">
         <v>56</v>
       </c>
@@ -2194,13 +2194,13 @@
         <v>33</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E63" s="10" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="64" spans="2:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B64" s="17">
         <v>57</v>
       </c>
@@ -2214,7 +2214,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="65" spans="2:5" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:5" s="1" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="B65" s="17">
         <v>58</v>
       </c>
@@ -2228,7 +2228,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="66" spans="2:5" s="1" customFormat="1" ht="72" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:5" s="1" customFormat="1" ht="69.599999999999994" x14ac:dyDescent="0.3">
       <c r="B66" s="17">
         <v>59</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="67" spans="2:5" s="1" customFormat="1" ht="72" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:5" s="1" customFormat="1" ht="69.599999999999994" x14ac:dyDescent="0.3">
       <c r="B67" s="17">
         <v>60</v>
       </c>
@@ -2256,7 +2256,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="68" spans="2:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B68" s="17">
         <v>61</v>
       </c>
@@ -2270,7 +2270,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="69" spans="2:5" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:5" s="1" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="B69" s="17">
         <v>62</v>
       </c>
@@ -2284,7 +2284,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="70" spans="2:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B70" s="17">
         <v>63</v>
       </c>
@@ -2298,7 +2298,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="71" spans="2:5" s="1" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:5" s="1" customFormat="1" ht="52.2" x14ac:dyDescent="0.3">
       <c r="B71" s="17">
         <v>64</v>
       </c>
@@ -2312,7 +2312,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="72" spans="2:5" s="1" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:5" s="1" customFormat="1" ht="52.2" x14ac:dyDescent="0.3">
       <c r="B72" s="17">
         <v>65</v>
       </c>
@@ -2326,16 +2326,16 @@
         <v>130</v>
       </c>
     </row>
-    <row r="75" spans="2:5" s="2" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:5" s="2" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="17"/>
       <c r="C75" s="3"/>
       <c r="D75" s="8"/>
       <c r="E75" s="3"/>
     </row>
-    <row r="78" spans="2:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C78" s="6"/>
     </row>
-    <row r="80" spans="2:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C80" s="6"/>
     </row>
   </sheetData>

</xml_diff>